<commit_message>
tidy up for rmd
</commit_message>
<xml_diff>
--- a/internal_datamap_files/risk_factor_plot_liftover.xlsx
+++ b/internal_datamap_files/risk_factor_plot_liftover.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7560A6C0-DA1F-314F-940D-76E41F13C487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B65FBD-630C-814F-ADF0-1898C767D787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="1880" windowWidth="21920" windowHeight="13580" xr2:uid="{7AA22FB0-B30D-7443-85DF-982F00AAE28F}"/>
   </bookViews>
@@ -32,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
-    <t>Urbanicity</t>
-  </si>
-  <si>
     <t>urban_rura_fctb</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>malaria intervention</t>
+  </si>
+  <si>
+    <t>Urbanicity (Rur.)</t>
   </si>
 </sst>
 </file>
@@ -233,24 +233,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -282,6 +264,24 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -296,15 +296,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8310AA48-1BEE-EE43-BF9C-2A2B75DE4867}" name="Table2" displayName="Table2" ref="A1:C14" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8310AA48-1BEE-EE43-BF9C-2A2B75DE4867}" name="Table2" displayName="Table2" ref="A1:C14" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C14" xr:uid="{4C92BE3E-2D72-7943-AFF5-C9EBB6188E3D}"/>
   <sortState ref="A2:C14">
     <sortCondition ref="C1:C14"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{596A1E9C-7A1B-4345-B763-FE8363FE4C8D}" name="target" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{37E8998A-76FA-A44E-8BD1-755A514FFFB9}" name="label" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{10AFD163-7EA4-F44B-A912-581F532BE19F}" name="group" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{596A1E9C-7A1B-4345-B763-FE8363FE4C8D}" name="target" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{37E8998A-76FA-A44E-8BD1-755A514FFFB9}" name="label" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{10AFD163-7EA4-F44B-A912-581F532BE19F}" name="group" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -610,7 +610,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,156 +622,156 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update temp and weather extract raster
</commit_message>
<xml_diff>
--- a/internal_datamap_files/risk_factor_plot_liftover.xlsx
+++ b/internal_datamap_files/risk_factor_plot_liftover.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B65FBD-630C-814F-ADF0-1898C767D787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33F4A14-3F4C-8D48-AE22-93725B7EE668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="1880" windowWidth="21920" windowHeight="13580" xr2:uid="{7AA22FB0-B30D-7443-85DF-982F00AAE28F}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>Wealth</t>
   </si>
   <si>
-    <t>hv108_cont_scale</t>
-  </si>
-  <si>
     <t>Education</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>Urbanicity (Rur.)</t>
+  </si>
+  <si>
+    <t>hv106_fctb</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,13 +622,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -639,7 +639,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -650,7 +650,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -661,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -672,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -683,7 +683,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -721,10 +721,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -738,18 +738,18 @@
         <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -757,10 +757,10 @@
         <v>0</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -771,7 +771,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update iptw health distance
</commit_message>
<xml_diff>
--- a/internal_datamap_files/risk_factor_plot_liftover.xlsx
+++ b/internal_datamap_files/risk_factor_plot_liftover.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD59FF9-E0D7-4445-BEFC-7C66DBE98B36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425600C7-49CF-104D-BDC0-DCDF50921F4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="1880" windowWidth="21920" windowHeight="13580" xr2:uid="{7AA22FB0-B30D-7443-85DF-982F00AAE28F}"/>
   </bookViews>
@@ -20,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -50,9 +45,6 @@
     <t>Water Dist.</t>
   </si>
   <si>
-    <t>hlthst_duration_fctb_clst</t>
-  </si>
-  <si>
     <t>Hospital Dist.</t>
   </si>
   <si>
@@ -138,6 +130,9 @@
   </si>
   <si>
     <t>Education (Lower)</t>
+  </si>
+  <si>
+    <t>hlthst_duration_cont_log_scale_clst</t>
   </si>
 </sst>
 </file>
@@ -304,7 +299,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8310AA48-1BEE-EE43-BF9C-2A2B75DE4867}" name="Table2" displayName="Table2" ref="A1:C15" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C15" xr:uid="{4C92BE3E-2D72-7943-AFF5-C9EBB6188E3D}"/>
-  <sortState ref="A2:C15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C15">
     <sortCondition ref="C1:C15"/>
   </sortState>
   <tableColumns count="3">
@@ -616,7 +611,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -628,35 +623,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -667,18 +662,18 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -689,84 +684,84 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -774,21 +769,21 @@
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update misc for hlth raster
</commit_message>
<xml_diff>
--- a/internal_datamap_files/risk_factor_plot_liftover.xlsx
+++ b/internal_datamap_files/risk_factor_plot_liftover.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425600C7-49CF-104D-BDC0-DCDF50921F4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701C0DEC-BCA5-644D-8B1B-48E83EA72C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="1880" windowWidth="21920" windowHeight="13580" xr2:uid="{7AA22FB0-B30D-7443-85DF-982F00AAE28F}"/>
+    <workbookView xWindow="1060" yWindow="7780" windowWidth="21920" windowHeight="13580" xr2:uid="{7AA22FB0-B30D-7443-85DF-982F00AAE28F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -132,7 +132,7 @@
     <t>Education (Lower)</t>
   </si>
   <si>
-    <t>hlthst_duration_cont_log_scale_clst</t>
+    <t>hlthdist_fctb_clst</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update for hlthdist and make temp simple weights
</commit_message>
<xml_diff>
--- a/internal_datamap_files/risk_factor_plot_liftover.xlsx
+++ b/internal_datamap_files/risk_factor_plot_liftover.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701C0DEC-BCA5-644D-8B1B-48E83EA72C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1080038-A656-1C41-A91E-7A592C83A396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="7780" windowWidth="21920" windowHeight="13580" xr2:uid="{7AA22FB0-B30D-7443-85DF-982F00AAE28F}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="21920" windowHeight="13580" xr2:uid="{7AA22FB0-B30D-7443-85DF-982F00AAE28F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
update model internal files
</commit_message>
<xml_diff>
--- a/internal_datamap_files/risk_factor_plot_liftover.xlsx
+++ b/internal_datamap_files/risk_factor_plot_liftover.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/internal_datamap_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA7678E-224A-6242-B152-E7AB4CE79562}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DFFE46-064B-E94A-BA16-33863AD9E9E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6700" yWindow="460" windowWidth="21920" windowHeight="13580" xr2:uid="{7AA22FB0-B30D-7443-85DF-982F00AAE28F}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>Housing Materials (Trad.)</t>
   </si>
   <si>
-    <t>wlthrcde_combscor_cont</t>
-  </si>
-  <si>
     <t>Wealth</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Hospital Dist. (Far)</t>
+  </si>
+  <si>
+    <t>wlthrcde_fctb</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,13 +623,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -640,7 +640,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -651,7 +651,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -662,18 +662,18 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -684,18 +684,18 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -722,10 +722,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>6</v>
@@ -733,10 +733,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>6</v>
@@ -750,18 +750,18 @@
         <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -769,21 +769,21 @@
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>